<commit_message>
Iteration3: Done, except PIP
</commit_message>
<xml_diff>
--- a/Iteration2/TimeLog-Iteration2.xlsx
+++ b/Iteration2/TimeLog-Iteration2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nil0310\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{2D2FC3B4-A91D-4287-8135-CC5D5E3FD44D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{15FA018B-8142-4B68-8C67-2AE65841708B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB140FD-607B-469E-8DD9-9762A599EC5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
   <si>
     <t>PSP Time Recording Log</t>
   </si>
@@ -367,6 +367,117 @@
   </si>
   <si>
     <t>Game Two</t>
+  </si>
+  <si>
+    <t>1:01pm</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>2:13pm</t>
+  </si>
+  <si>
+    <t>2:21pm</t>
+  </si>
+  <si>
+    <t>2:37pm</t>
+  </si>
+  <si>
+    <t>2:40pm</t>
+  </si>
+  <si>
+    <t>11:02am</t>
+  </si>
+  <si>
+    <t>11:07am</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>2:23pm</t>
+  </si>
+  <si>
+    <t>2:32pm</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>3:16pm</t>
+  </si>
+  <si>
+    <t>3:21pm</t>
+  </si>
+  <si>
+    <t>3:31pm</t>
+  </si>
+  <si>
+    <t>3:35pm</t>
+  </si>
+  <si>
+    <t>3:42pm</t>
+  </si>
+  <si>
+    <t>3:48pm</t>
+  </si>
+  <si>
+    <t>4:22pm</t>
+  </si>
+  <si>
+    <t>4:31pm</t>
+  </si>
+  <si>
+    <t>4:36pm</t>
+  </si>
+  <si>
+    <t>4:53pm</t>
+  </si>
+  <si>
+    <t>6:55pm</t>
+  </si>
+  <si>
+    <t>7:05pm</t>
+  </si>
+  <si>
+    <t>10:46am</t>
+  </si>
+  <si>
+    <t>10:56am</t>
+  </si>
+  <si>
+    <t>10:13am</t>
+  </si>
+  <si>
+    <t>10:19am</t>
+  </si>
+  <si>
+    <t>10:57am</t>
+  </si>
+  <si>
+    <t>Preliminary designs</t>
+  </si>
+  <si>
+    <t>Write tests</t>
+  </si>
+  <si>
+    <t>More design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code </t>
+  </si>
+  <si>
+    <t>Test code</t>
+  </si>
+  <si>
+    <t>Fix code</t>
+  </si>
+  <si>
+    <t>Test again</t>
+  </si>
+  <si>
+    <t>Fix designs</t>
   </si>
 </sst>
 </file>
@@ -976,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,8 +1172,232 @@
       <c r="D7" s="14" t="s">
         <v>39</v>
       </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
       <c r="H7" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="14">
+        <v>43558</v>
+      </c>
+      <c r="D16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="14">
+        <v>43559</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="14">
+        <v>43559</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="14">
+        <v>43559</v>
+      </c>
+      <c r="D19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="14">
+        <v>43559</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>